<commit_message>
refactored sample hough file names
</commit_message>
<xml_diff>
--- a/doc/hough created.xlsx
+++ b/doc/hough created.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushn\projects\cv-workbench\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D2C52E-55D0-47D9-BC82-63CB4A9A25DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8248F74C-5C46-4BE5-AEAC-1E42BF5FEACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EEFBBBD4-DAC4-4F35-8600-CC9D3F6E2E33}"/>
+    <workbookView xWindow="1416" yWindow="192" windowWidth="20508" windowHeight="11688" xr2:uid="{EEFBBBD4-DAC4-4F35-8600-CC9D3F6E2E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>ncols</t>
   </si>
@@ -201,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -392,24 +392,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -447,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -462,28 +444,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944A79A4-ED4E-4E71-8792-EA1E8F7DCD63}">
-  <dimension ref="A4:AQ35"/>
+  <dimension ref="A5:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,47 +820,7 @@
     <col min="44" max="46" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="K5">
-        <f t="shared" ref="H5:V7" si="0">K6-$X$6+0.5</f>
-        <v>-3.5</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5" si="1">L6-$X$6+0.5</f>
-        <v>-2.5</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5" si="2">M6-$X$6+0.5</f>
-        <v>-1.5</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5" si="3">N6-$X$6+0.5</f>
-        <v>-0.5</v>
-      </c>
-      <c r="O5">
-        <f t="shared" ref="O5" si="4">O6-$X$6+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="P5">
-        <f t="shared" ref="P5" si="5">P6-$X$6+0.5</f>
-        <v>1.5</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5" si="6">Q6-$X$6+0.5</f>
-        <v>2.5</v>
-      </c>
-      <c r="R5">
-        <f t="shared" ref="R5" si="7">R6-$X$6+0.5</f>
-        <v>3.5</v>
-      </c>
       <c r="W5" t="s">
         <v>0</v>
       </c>
@@ -911,31 +852,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K6" s="15">
-        <v>0</v>
-      </c>
-      <c r="L6" s="15">
-        <v>1</v>
-      </c>
-      <c r="M6" s="15">
-        <v>2</v>
-      </c>
-      <c r="N6" s="15">
-        <v>3</v>
-      </c>
-      <c r="O6" s="15">
-        <v>4</v>
-      </c>
-      <c r="P6" s="15">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="15">
-        <v>6</v>
-      </c>
-      <c r="R6" s="15">
-        <v>7</v>
-      </c>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
       <c r="W6" t="s">
         <v>1</v>
       </c>
@@ -943,7 +868,7 @@
         <f>X5/2</f>
         <v>4</v>
       </c>
-      <c r="Z6" s="18" t="s">
+      <c r="Z6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AB6">
@@ -968,13 +893,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="G7">
         <f>G8-$X$6+0.5</f>
         <v>-3.5</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H5:V7" si="0">H8-$X$6+0.5</f>
         <v>-2.5</v>
       </c>
       <c r="I7">
@@ -1036,32 +961,32 @@
       <c r="Z7" t="s">
         <v>11</v>
       </c>
-      <c r="AB7" s="19">
+      <c r="AB7" s="17">
         <f>AB6*3.14159/180</f>
         <v>0.52359833333333328</v>
       </c>
-      <c r="AC7" s="19">
-        <f t="shared" ref="AC7:AH7" si="8">AC6*3.14159/180</f>
+      <c r="AC7" s="17">
+        <f t="shared" ref="AC7:AH7" si="1">AC6*3.14159/180</f>
         <v>0.61086472222222221</v>
       </c>
-      <c r="AD7" s="19">
-        <f t="shared" si="8"/>
+      <c r="AD7" s="17">
+        <f t="shared" si="1"/>
         <v>0.69813111111111115</v>
       </c>
-      <c r="AE7" s="19">
-        <f t="shared" si="8"/>
+      <c r="AE7" s="17">
+        <f t="shared" si="1"/>
         <v>0.78539749999999997</v>
       </c>
-      <c r="AF7" s="19">
-        <f t="shared" si="8"/>
+      <c r="AF7" s="17">
+        <f t="shared" si="1"/>
         <v>0.87266388888888891</v>
       </c>
-      <c r="AG7" s="23">
-        <f t="shared" si="8"/>
+      <c r="AG7" s="21">
+        <f t="shared" si="1"/>
         <v>0.95993027777777784</v>
       </c>
-      <c r="AH7" s="23">
-        <f t="shared" si="8"/>
+      <c r="AH7" s="21">
+        <f t="shared" si="1"/>
         <v>1.0471966666666666</v>
       </c>
     </row>
@@ -1117,32 +1042,32 @@
       <c r="Z8" t="s">
         <v>9</v>
       </c>
-      <c r="AB8" s="28">
+      <c r="AB8" s="26">
         <f>COS(AB7)</f>
         <v>0.86602562491683677</v>
       </c>
       <c r="AC8">
-        <f t="shared" ref="AC8:AH8" si="9">COS(AC7)</f>
+        <f t="shared" ref="AC8:AH8" si="2">COS(AC7)</f>
         <v>0.81915234024043937</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0.76604482216209824</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0.70710725027922627</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>0.64278817434406343</v>
       </c>
-      <c r="AG8" s="20">
-        <f t="shared" si="9"/>
+      <c r="AG8" s="18">
+        <f t="shared" si="2"/>
         <v>0.57357710053498367</v>
       </c>
-      <c r="AH8" s="20">
-        <f t="shared" si="9"/>
+      <c r="AH8" s="18">
+        <f t="shared" si="2"/>
         <v>0.50000076602519528</v>
       </c>
       <c r="AJ8" t="s">
@@ -1157,7 +1082,7 @@
       <c r="AM8">
         <v>2</v>
       </c>
-      <c r="AN8" s="35">
+      <c r="AN8" s="33">
         <v>3</v>
       </c>
       <c r="AO8">
@@ -1203,35 +1128,35 @@
       <c r="Z9" t="s">
         <v>10</v>
       </c>
-      <c r="AB9" s="29">
+      <c r="AB9" s="27">
         <f>SIN(AB7)</f>
         <v>0.4999996169872557</v>
       </c>
-      <c r="AC9" s="19">
-        <f t="shared" ref="AC9:AH9" si="10">SIN(AC7)</f>
+      <c r="AC9" s="17">
+        <f t="shared" ref="AC9:AH9" si="3">SIN(AC7)</f>
         <v>0.57357601368834399</v>
       </c>
-      <c r="AD9" s="19">
-        <f t="shared" si="10"/>
+      <c r="AD9" s="17">
+        <f t="shared" si="3"/>
         <v>0.64278715796026864</v>
       </c>
-      <c r="AE9" s="19">
-        <f t="shared" si="10"/>
+      <c r="AE9" s="17">
+        <f t="shared" si="3"/>
         <v>0.70710631209355757</v>
       </c>
-      <c r="AF9" s="19">
-        <f t="shared" si="10"/>
+      <c r="AF9" s="17">
+        <f t="shared" si="3"/>
         <v>0.7660439693147032</v>
       </c>
-      <c r="AG9" s="23">
-        <f t="shared" si="10"/>
+      <c r="AG9" s="21">
+        <f t="shared" si="3"/>
         <v>0.81915157922199067</v>
       </c>
-      <c r="AH9" s="23">
-        <f t="shared" si="10"/>
+      <c r="AH9" s="21">
+        <f t="shared" si="3"/>
         <v>0.86602496151913422</v>
       </c>
-      <c r="AJ9" s="18" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>8</v>
       </c>
       <c r="AK9">
@@ -1243,7 +1168,7 @@
       <c r="AM9">
         <v>40</v>
       </c>
-      <c r="AN9" s="35">
+      <c r="AN9" s="33">
         <v>45</v>
       </c>
       <c r="AO9">
@@ -1265,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="C10:E24" si="11">$B$10-F10-0.5</f>
+        <f t="shared" ref="E10:E24" si="4">$B$10-F10-0.5</f>
         <v>2.5</v>
       </c>
       <c r="F10">
@@ -1287,35 +1212,35 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="X10" s="19" t="s">
+      <c r="X10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Y10" s="19" t="s">
+      <c r="Y10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Z10" s="24" t="s">
+      <c r="Z10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AA10" s="19" t="s">
+      <c r="AA10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AB10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="19"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+      <c r="AG10" s="17"/>
+      <c r="AH10" s="17"/>
       <c r="AJ10" t="s">
         <v>34</v>
       </c>
-      <c r="AN10" s="35"/>
+      <c r="AN10" s="33"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="E11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="F11">
@@ -1325,14 +1250,38 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="K11" s="1">
+        <f>-($B$10-K12-0.5)</f>
+        <v>-3.5</v>
+      </c>
+      <c r="L11" s="1">
+        <f>K11+1</f>
+        <v>-2.5</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" ref="M11:R11" si="5">L11+1</f>
+        <v>-1.5</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.5</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1343,74 +1292,74 @@
       <c r="Y11">
         <v>2</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="24">
         <f>X11-$X$6+0.5</f>
         <v>-3.5</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AA11" s="25">
         <f>$B$10-Y11-0.5</f>
         <v>1.5</v>
       </c>
-      <c r="AB11" s="30">
+      <c r="AB11" s="28">
         <f>$Z11*AB$8+$AA11*AB$9</f>
         <v>-2.2810902617280453</v>
       </c>
-      <c r="AC11" s="30">
-        <f t="shared" ref="AC11:AH16" si="12">$Z11*AC$8+$AA11*AC$9</f>
+      <c r="AC11" s="28">
+        <f t="shared" ref="AC11:AH16" si="6">$Z11*AC$8+$AA11*AC$9</f>
         <v>-2.0066691703090216</v>
       </c>
-      <c r="AD11" s="30">
-        <f t="shared" si="12"/>
+      <c r="AD11" s="28">
+        <f t="shared" si="6"/>
         <v>-1.7169761406269408</v>
       </c>
-      <c r="AE11" s="30">
-        <f t="shared" si="12"/>
+      <c r="AE11" s="28">
+        <f t="shared" si="6"/>
         <v>-1.4142159078369556</v>
       </c>
-      <c r="AF11" s="30">
-        <f t="shared" si="12"/>
+      <c r="AF11" s="28">
+        <f t="shared" si="6"/>
         <v>-1.1006926562321673</v>
       </c>
-      <c r="AG11" s="30">
-        <f t="shared" si="12"/>
+      <c r="AG11" s="28">
+        <f t="shared" si="6"/>
         <v>-0.77879248303945703</v>
       </c>
-      <c r="AH11" s="30">
-        <f t="shared" si="12"/>
+      <c r="AH11" s="28">
+        <f t="shared" si="6"/>
         <v>-0.45096523880948203</v>
       </c>
-      <c r="AK11" s="20">
+      <c r="AK11" s="18">
         <f>($AG$23-1)*(AB11-$AG$22)/$AG$20</f>
         <v>-1.9894280465094287E-5</v>
       </c>
-      <c r="AL11" s="20">
-        <f t="shared" ref="AL11:AL16" si="13">($AG$23-1)*(AC11-$AG$22)/$AG$20</f>
+      <c r="AL11" s="18">
+        <f t="shared" ref="AL11:AL16" si="7">($AG$23-1)*(AC11-$AG$22)/$AG$20</f>
         <v>1.349499117306564</v>
       </c>
-      <c r="AM11" s="20">
-        <f t="shared" ref="AM11:AM16" si="14">($AG$23-1)*(AD11-$AG$22)/$AG$20</f>
+      <c r="AM11" s="18">
+        <f t="shared" ref="AM11:AM16" si="8">($AG$23-1)*(AD11-$AG$22)/$AG$20</f>
         <v>2.7741208512215536</v>
       </c>
-      <c r="AN11" s="34">
-        <f t="shared" ref="AN11:AN16" si="15">($AG$23-1)*(AE11-$AG$22)/$AG$20</f>
+      <c r="AN11" s="32">
+        <f t="shared" ref="AN11:AN16" si="9">($AG$23-1)*(AE11-$AG$22)/$AG$20</f>
         <v>4.2630030941637438</v>
       </c>
-      <c r="AO11" s="20">
-        <f t="shared" ref="AO11:AO16" si="16">($AG$23-1)*(AF11-$AG$22)/$AG$20</f>
+      <c r="AO11" s="18">
+        <f t="shared" ref="AO11:AO16" si="10">($AG$23-1)*(AF11-$AG$22)/$AG$20</f>
         <v>5.8048145723827771</v>
       </c>
-      <c r="AP11" s="20">
-        <f t="shared" ref="AP11:AP16" si="17">($AG$23-1)*(AG11-$AG$22)/$AG$20</f>
+      <c r="AP11" s="18">
+        <f t="shared" ref="AP11:AP16" si="11">($AG$23-1)*(AG11-$AG$22)/$AG$20</f>
         <v>7.3878211893683581</v>
       </c>
-      <c r="AQ11" s="20">
-        <f t="shared" ref="AQ11:AQ16" si="18">($AG$23-1)*(AH11-$AG$22)/$AG$20</f>
+      <c r="AQ11" s="18">
+        <f t="shared" ref="AQ11:AQ16" si="12">($AG$23-1)*(AH11-$AG$22)/$AG$20</f>
         <v>8.9999753292591738</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="F12">
@@ -1420,14 +1369,30 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
+        <v>2</v>
+      </c>
+      <c r="N12" s="4">
+        <v>3</v>
+      </c>
+      <c r="O12" s="4">
+        <v>4</v>
+      </c>
+      <c r="P12" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>6</v>
+      </c>
+      <c r="R12" s="4">
+        <v>7</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1438,68 +1403,68 @@
       <c r="Y12">
         <v>3</v>
       </c>
-      <c r="Z12" s="22">
-        <f t="shared" ref="Z12:Z16" si="19">X12-$X$6+0.5</f>
+      <c r="Z12" s="20">
+        <f t="shared" ref="Z12:Z16" si="13">X12-$X$6+0.5</f>
         <v>-2.5</v>
       </c>
-      <c r="AA12" s="21">
-        <f t="shared" ref="AA12:AA16" si="20">$B$10-Y12-0.5</f>
+      <c r="AA12" s="19">
+        <f t="shared" ref="AA12:AA16" si="14">$B$10-Y12-0.5</f>
         <v>0.5</v>
       </c>
-      <c r="AB12" s="30">
-        <f t="shared" ref="AB12:AB16" si="21">$Z12*AB$8+$AA12*AB$9</f>
+      <c r="AB12" s="28">
+        <f t="shared" ref="AB12:AB16" si="15">$Z12*AB$8+$AA12*AB$9</f>
         <v>-1.9150642537984641</v>
       </c>
-      <c r="AC12" s="30">
+      <c r="AC12" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.7610928437569267</v>
+      </c>
+      <c r="AD12" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.5937184764251113</v>
+      </c>
+      <c r="AE12" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4142149696512869</v>
+      </c>
+      <c r="AF12" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.2239484512028072</v>
+      </c>
+      <c r="AG12" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.0243669617264639</v>
+      </c>
+      <c r="AH12" s="28">
+        <f t="shared" si="6"/>
+        <v>-0.81698943430342108</v>
+      </c>
+      <c r="AK12" s="18">
+        <f t="shared" ref="AK12:AK16" si="16">($AG$23-1)*(AB12-$AG$22)/$AG$20</f>
+        <v>1.7999840845756283</v>
+      </c>
+      <c r="AL12" s="18">
+        <f t="shared" si="7"/>
+        <v>2.5571683958013232</v>
+      </c>
+      <c r="AM12" s="18">
+        <f t="shared" si="8"/>
+        <v>3.3802643524518965</v>
+      </c>
+      <c r="AN12" s="32">
+        <f t="shared" si="9"/>
+        <v>4.2630077078739719</v>
+      </c>
+      <c r="AO12" s="18">
+        <f t="shared" si="10"/>
+        <v>5.1986802634598268</v>
+      </c>
+      <c r="AP12" s="18">
+        <f t="shared" si="11"/>
+        <v>6.1801609981090389</v>
+      </c>
+      <c r="AQ12" s="18">
         <f t="shared" si="12"/>
-        <v>-1.7610928437569267</v>
-      </c>
-      <c r="AD12" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.5937184764251113</v>
-      </c>
-      <c r="AE12" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4142149696512869</v>
-      </c>
-      <c r="AF12" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.2239484512028072</v>
-      </c>
-      <c r="AG12" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.0243669617264639</v>
-      </c>
-      <c r="AH12" s="30">
-        <f t="shared" si="12"/>
-        <v>-0.81698943430342108</v>
-      </c>
-      <c r="AK12" s="20">
-        <f t="shared" ref="AK12:AK16" si="22">($AG$23-1)*(AB12-$AG$22)/$AG$20</f>
-        <v>1.7999840845756283</v>
-      </c>
-      <c r="AL12" s="20">
-        <f t="shared" si="13"/>
-        <v>2.5571683958013232</v>
-      </c>
-      <c r="AM12" s="20">
-        <f t="shared" si="14"/>
-        <v>3.3802643524518965</v>
-      </c>
-      <c r="AN12" s="34">
-        <f t="shared" si="15"/>
-        <v>4.2630077078739719</v>
-      </c>
-      <c r="AO12" s="20">
-        <f t="shared" si="16"/>
-        <v>5.1986802634598268</v>
-      </c>
-      <c r="AP12" s="20">
-        <f t="shared" si="17"/>
-        <v>6.1801609981090389</v>
-      </c>
-      <c r="AQ12" s="20">
-        <f t="shared" si="18"/>
         <v>7.1999802634073387</v>
       </c>
     </row>
@@ -1507,15 +1472,8 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
-        <f>$B$10-D13-0.5</f>
-        <v>3.5</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
       <c r="E13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-0.5</v>
       </c>
       <c r="F13">
@@ -1523,8 +1481,13 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
+      <c r="I13" s="1">
+        <f>$B$10-J13-0.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
       <c r="K13" s="6"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -1543,81 +1506,74 @@
       <c r="Y13">
         <v>4</v>
       </c>
-      <c r="Z13" s="22">
-        <f t="shared" si="19"/>
+      <c r="Z13" s="20">
+        <f t="shared" si="13"/>
         <v>-1.5</v>
       </c>
-      <c r="AA13" s="21">
-        <f t="shared" si="20"/>
+      <c r="AA13" s="19">
+        <f t="shared" si="14"/>
         <v>-0.5</v>
       </c>
-      <c r="AB13" s="30">
-        <f t="shared" si="21"/>
+      <c r="AB13" s="28">
+        <f t="shared" si="15"/>
         <v>-1.5490382458688829</v>
       </c>
-      <c r="AC13" s="30">
+      <c r="AC13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.515516517204831</v>
+      </c>
+      <c r="AD13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4704608122232816</v>
+      </c>
+      <c r="AE13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4142140314656182</v>
+      </c>
+      <c r="AF13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.3472042461734466</v>
+      </c>
+      <c r="AG13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.2699414404134708</v>
+      </c>
+      <c r="AH13" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.1830136297973599</v>
+      </c>
+      <c r="AK13" s="18">
+        <f t="shared" si="16"/>
+        <v>3.5999880634317218</v>
+      </c>
+      <c r="AL13" s="18">
+        <f t="shared" si="7"/>
+        <v>3.7648376742960852</v>
+      </c>
+      <c r="AM13" s="18">
+        <f t="shared" si="8"/>
+        <v>3.9864078536822394</v>
+      </c>
+      <c r="AN13" s="32">
+        <f t="shared" si="9"/>
+        <v>4.2630123215842</v>
+      </c>
+      <c r="AO13" s="18">
+        <f t="shared" si="10"/>
+        <v>4.5925459545368801</v>
+      </c>
+      <c r="AP13" s="18">
+        <f t="shared" si="11"/>
+        <v>4.9725008068497187</v>
+      </c>
+      <c r="AQ13" s="18">
         <f t="shared" si="12"/>
-        <v>-1.515516517204831</v>
-      </c>
-      <c r="AD13" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4704608122232816</v>
-      </c>
-      <c r="AE13" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4142140314656182</v>
-      </c>
-      <c r="AF13" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.3472042461734466</v>
-      </c>
-      <c r="AG13" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.2699414404134708</v>
-      </c>
-      <c r="AH13" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.1830136297973599</v>
-      </c>
-      <c r="AK13" s="20">
-        <f t="shared" si="22"/>
-        <v>3.5999880634317218</v>
-      </c>
-      <c r="AL13" s="20">
-        <f t="shared" si="13"/>
-        <v>3.7648376742960852</v>
-      </c>
-      <c r="AM13" s="20">
-        <f t="shared" si="14"/>
-        <v>3.9864078536822394</v>
-      </c>
-      <c r="AN13" s="34">
-        <f t="shared" si="15"/>
-        <v>4.2630123215842</v>
-      </c>
-      <c r="AO13" s="20">
-        <f t="shared" si="16"/>
-        <v>4.5925459545368801</v>
-      </c>
-      <c r="AP13" s="20">
-        <f t="shared" si="17"/>
-        <v>4.9725008068497187</v>
-      </c>
-      <c r="AQ13" s="20">
-        <f t="shared" si="18"/>
         <v>5.3999851975555053</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C14">
-        <f t="shared" si="11"/>
-        <v>2.5</v>
-      </c>
-      <c r="D14" s="14">
-        <v>1</v>
-      </c>
       <c r="E14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-1.5</v>
       </c>
       <c r="F14">
@@ -1625,8 +1581,13 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14:I20" si="17">$B$10-J14-0.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1645,81 +1606,74 @@
       <c r="Y14">
         <v>5</v>
       </c>
-      <c r="Z14" s="22">
-        <f t="shared" si="19"/>
+      <c r="Z14" s="20">
+        <f t="shared" si="13"/>
         <v>-0.5</v>
       </c>
-      <c r="AA14" s="21">
-        <f t="shared" si="20"/>
+      <c r="AA14" s="19">
+        <f t="shared" si="14"/>
         <v>-1.5</v>
       </c>
-      <c r="AB14" s="30">
-        <f t="shared" si="21"/>
+      <c r="AB14" s="28">
+        <f t="shared" si="15"/>
         <v>-1.1830122379393018</v>
       </c>
-      <c r="AC14" s="30">
+      <c r="AC14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.2699401906527357</v>
+      </c>
+      <c r="AD14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.3472031480214521</v>
+      </c>
+      <c r="AE14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4142130932799495</v>
+      </c>
+      <c r="AF14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4704600411440867</v>
+      </c>
+      <c r="AG14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.5155159191004779</v>
+      </c>
+      <c r="AH14" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.5490378252912991</v>
+      </c>
+      <c r="AK14" s="18">
+        <f t="shared" si="16"/>
+        <v>5.399992042287816</v>
+      </c>
+      <c r="AL14" s="18">
+        <f t="shared" si="7"/>
+        <v>4.9725069527908463</v>
+      </c>
+      <c r="AM14" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5925513549125814</v>
+      </c>
+      <c r="AN14" s="32">
+        <f t="shared" si="9"/>
+        <v>4.263016935294428</v>
+      </c>
+      <c r="AO14" s="18">
+        <f t="shared" si="10"/>
+        <v>3.9864116456139298</v>
+      </c>
+      <c r="AP14" s="18">
+        <f t="shared" si="11"/>
+        <v>3.7648406155903977</v>
+      </c>
+      <c r="AQ14" s="18">
         <f t="shared" si="12"/>
-        <v>-1.2699401906527357</v>
-      </c>
-      <c r="AD14" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.3472031480214521</v>
-      </c>
-      <c r="AE14" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4142130932799495</v>
-      </c>
-      <c r="AF14" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4704600411440867</v>
-      </c>
-      <c r="AG14" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.5155159191004779</v>
-      </c>
-      <c r="AH14" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.5490378252912991</v>
-      </c>
-      <c r="AK14" s="20">
-        <f t="shared" si="22"/>
-        <v>5.399992042287816</v>
-      </c>
-      <c r="AL14" s="20">
-        <f t="shared" si="13"/>
-        <v>4.9725069527908463</v>
-      </c>
-      <c r="AM14" s="20">
-        <f t="shared" si="14"/>
-        <v>4.5925513549125814</v>
-      </c>
-      <c r="AN14" s="34">
-        <f t="shared" si="15"/>
-        <v>4.263016935294428</v>
-      </c>
-      <c r="AO14" s="20">
-        <f t="shared" si="16"/>
-        <v>3.9864116456139298</v>
-      </c>
-      <c r="AP14" s="20">
-        <f t="shared" si="17"/>
-        <v>3.7648406155903977</v>
-      </c>
-      <c r="AQ14" s="20">
-        <f t="shared" si="18"/>
         <v>3.5999901317036693</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C15">
-        <f t="shared" si="11"/>
-        <v>1.5</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2</v>
-      </c>
       <c r="E15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-2.5</v>
       </c>
       <c r="F15">
@@ -1727,9 +1681,14 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="16"/>
+      <c r="I15" s="1">
+        <f t="shared" si="17"/>
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="14"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1747,81 +1706,74 @@
       <c r="Y15">
         <v>6</v>
       </c>
-      <c r="Z15" s="22">
-        <f t="shared" si="19"/>
+      <c r="Z15" s="20">
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="AA15" s="21">
-        <f t="shared" si="20"/>
+      <c r="AA15" s="19">
+        <f t="shared" si="14"/>
         <v>-2.5</v>
       </c>
-      <c r="AB15" s="30">
-        <f t="shared" si="21"/>
+      <c r="AB15" s="28">
+        <f t="shared" si="15"/>
         <v>-0.81698623000972093</v>
       </c>
-      <c r="AC15" s="30">
+      <c r="AC15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.0243638641006403</v>
+      </c>
+      <c r="AD15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.2239454838196224</v>
+      </c>
+      <c r="AE15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4142121550942808</v>
+      </c>
+      <c r="AF15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.5937158361147261</v>
+      </c>
+      <c r="AG15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.7610903977874848</v>
+      </c>
+      <c r="AH15" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.9150620207852378</v>
+      </c>
+      <c r="AK15" s="18">
+        <f t="shared" si="16"/>
+        <v>7.1999960211439067</v>
+      </c>
+      <c r="AL15" s="18">
+        <f t="shared" si="7"/>
+        <v>6.180176231285607</v>
+      </c>
+      <c r="AM15" s="18">
+        <f t="shared" si="8"/>
+        <v>5.1986948561429251</v>
+      </c>
+      <c r="AN15" s="32">
+        <f t="shared" si="9"/>
+        <v>4.2630215490046561</v>
+      </c>
+      <c r="AO15" s="18">
+        <f t="shared" si="10"/>
+        <v>3.3802773366909822</v>
+      </c>
+      <c r="AP15" s="18">
+        <f t="shared" si="11"/>
+        <v>2.5571804243310781</v>
+      </c>
+      <c r="AQ15" s="18">
         <f t="shared" si="12"/>
-        <v>-1.0243638641006403</v>
-      </c>
-      <c r="AD15" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.2239454838196224</v>
-      </c>
-      <c r="AE15" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4142121550942808</v>
-      </c>
-      <c r="AF15" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.5937158361147261</v>
-      </c>
-      <c r="AG15" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.7610903977874848</v>
-      </c>
-      <c r="AH15" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.9150620207852378</v>
-      </c>
-      <c r="AK15" s="20">
-        <f t="shared" si="22"/>
-        <v>7.1999960211439067</v>
-      </c>
-      <c r="AL15" s="20">
-        <f t="shared" si="13"/>
-        <v>6.180176231285607</v>
-      </c>
-      <c r="AM15" s="20">
-        <f t="shared" si="14"/>
-        <v>5.1986948561429251</v>
-      </c>
-      <c r="AN15" s="34">
-        <f t="shared" si="15"/>
-        <v>4.2630215490046561</v>
-      </c>
-      <c r="AO15" s="20">
-        <f t="shared" si="16"/>
-        <v>3.3802773366909822</v>
-      </c>
-      <c r="AP15" s="20">
-        <f t="shared" si="17"/>
-        <v>2.5571804243310781</v>
-      </c>
-      <c r="AQ15" s="20">
-        <f t="shared" si="18"/>
         <v>1.799995065851836</v>
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C16">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="14">
-        <v>3</v>
-      </c>
       <c r="E16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-3.5</v>
       </c>
       <c r="F16">
@@ -1829,10 +1781,15 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
+      <c r="I16" s="1">
+        <f t="shared" si="17"/>
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3</v>
+      </c>
       <c r="K16" s="9"/>
-      <c r="L16" s="17"/>
+      <c r="L16" s="15"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1850,81 +1807,74 @@
       <c r="Y16">
         <v>7</v>
       </c>
-      <c r="Z16" s="22">
-        <f t="shared" si="19"/>
+      <c r="Z16" s="20">
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
-      <c r="AA16" s="21">
-        <f t="shared" si="20"/>
+      <c r="AA16" s="19">
+        <f t="shared" si="14"/>
         <v>-3.5</v>
       </c>
-      <c r="AB16" s="30">
-        <f t="shared" si="21"/>
+      <c r="AB16" s="28">
+        <f t="shared" si="15"/>
         <v>-0.45096022208013986</v>
       </c>
-      <c r="AC16" s="30">
+      <c r="AC16" s="28">
+        <f t="shared" si="6"/>
+        <v>-0.77878753754854491</v>
+      </c>
+      <c r="AD16" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.1006878196177927</v>
+      </c>
+      <c r="AE16" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.4142112169086121</v>
+      </c>
+      <c r="AF16" s="28">
+        <f t="shared" si="6"/>
+        <v>-1.7169716310853662</v>
+      </c>
+      <c r="AG16" s="28">
+        <f t="shared" si="6"/>
+        <v>-2.0066648764744919</v>
+      </c>
+      <c r="AH16" s="28">
+        <f t="shared" si="6"/>
+        <v>-2.281086216279177</v>
+      </c>
+      <c r="AK16" s="18">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="AL16" s="18">
+        <f t="shared" si="7"/>
+        <v>7.3878455097803686</v>
+      </c>
+      <c r="AM16" s="18">
+        <f t="shared" si="8"/>
+        <v>5.8048383573732689</v>
+      </c>
+      <c r="AN16" s="32">
+        <f t="shared" si="9"/>
+        <v>4.2630261627148842</v>
+      </c>
+      <c r="AO16" s="18">
+        <f t="shared" si="10"/>
+        <v>2.7741430277680319</v>
+      </c>
+      <c r="AP16" s="18">
+        <f t="shared" si="11"/>
+        <v>1.3495202330717571</v>
+      </c>
+      <c r="AQ16" s="18">
         <f t="shared" si="12"/>
-        <v>-0.77878753754854491</v>
-      </c>
-      <c r="AD16" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.1006878196177927</v>
-      </c>
-      <c r="AE16" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.4142112169086121</v>
-      </c>
-      <c r="AF16" s="30">
-        <f t="shared" si="12"/>
-        <v>-1.7169716310853662</v>
-      </c>
-      <c r="AG16" s="30">
-        <f t="shared" si="12"/>
-        <v>-2.0066648764744919</v>
-      </c>
-      <c r="AH16" s="30">
-        <f t="shared" si="12"/>
-        <v>-2.281086216279177</v>
-      </c>
-      <c r="AK16" s="20">
-        <f t="shared" si="22"/>
-        <v>9</v>
-      </c>
-      <c r="AL16" s="20">
-        <f t="shared" si="13"/>
-        <v>7.3878455097803686</v>
-      </c>
-      <c r="AM16" s="20">
-        <f t="shared" si="14"/>
-        <v>5.8048383573732689</v>
-      </c>
-      <c r="AN16" s="34">
-        <f t="shared" si="15"/>
-        <v>4.2630261627148842</v>
-      </c>
-      <c r="AO16" s="20">
-        <f t="shared" si="16"/>
-        <v>2.7741430277680319</v>
-      </c>
-      <c r="AP16" s="20">
-        <f t="shared" si="17"/>
-        <v>1.3495202330717571</v>
-      </c>
-      <c r="AQ16" s="20">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C17">
-        <f t="shared" si="11"/>
-        <v>-0.5</v>
-      </c>
-      <c r="D17" s="14">
-        <v>4</v>
-      </c>
       <c r="E17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-4.5</v>
       </c>
       <c r="F17">
@@ -1932,11 +1882,16 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
+      <c r="I17" s="1">
+        <f t="shared" si="17"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="17"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1946,18 +1901,11 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="AN17" s="35"/>
+      <c r="AN17" s="33"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <f t="shared" si="11"/>
-        <v>-1.5</v>
-      </c>
-      <c r="D18" s="14">
-        <v>5</v>
-      </c>
       <c r="E18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-5.5</v>
       </c>
       <c r="F18">
@@ -1965,12 +1913,17 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
+      <c r="I18" s="1">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="17"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -1979,21 +1932,21 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-      <c r="X18" s="31" t="s">
+      <c r="X18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31">
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29">
         <v>30</v>
       </c>
       <c r="AE18" t="s">
         <v>25</v>
       </c>
-      <c r="AG18" s="20">
+      <c r="AG18" s="18">
         <f>AC24-AC22</f>
         <v>7</v>
       </c>
-      <c r="AI18" s="20">
+      <c r="AI18" s="18">
         <f>(AJ18*$AG$20) / ($AG$23 - 1) + $AG$22</f>
         <v>-2.281086216279177</v>
       </c>
@@ -2003,21 +1956,14 @@
       <c r="AK18">
         <v>1</v>
       </c>
-      <c r="AN18" s="35"/>
+      <c r="AN18" s="33"/>
       <c r="AQ18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <f t="shared" si="11"/>
-        <v>-2.5</v>
-      </c>
-      <c r="D19" s="14">
-        <v>6</v>
-      </c>
       <c r="E19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-6.5</v>
       </c>
       <c r="F19">
@@ -2025,13 +1971,18 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
+      <c r="I19" s="1">
+        <f t="shared" si="17"/>
+        <v>-2.5</v>
+      </c>
+      <c r="J19" s="2">
+        <v>6</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="17"/>
+      <c r="O19" s="15"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="10"/>
@@ -2039,22 +1990,22 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="X19" s="31" t="s">
+      <c r="X19" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="Y19" s="31"/>
-      <c r="Z19" s="31">
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29">
         <v>60</v>
       </c>
       <c r="AE19" t="s">
         <v>26</v>
       </c>
-      <c r="AG19" s="20">
+      <c r="AG19" s="18">
         <f>AC25-AC23</f>
         <v>-7</v>
       </c>
-      <c r="AI19" s="20">
-        <f t="shared" ref="AI19:AI27" si="23">(AJ19*$AG$20) / ($AG$23 - 1) + $AG$22</f>
+      <c r="AI19" s="18">
+        <f t="shared" ref="AI19:AI27" si="18">(AJ19*$AG$20) / ($AG$23 - 1) + $AG$22</f>
         <v>-2.0777388835903952</v>
       </c>
       <c r="AJ19">
@@ -2063,7 +2014,7 @@
       <c r="AL19">
         <v>1</v>
       </c>
-      <c r="AN19" s="35"/>
+      <c r="AN19" s="33"/>
       <c r="AP19">
         <v>1</v>
       </c>
@@ -2072,15 +2023,8 @@
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="11"/>
-        <v>-3.5</v>
-      </c>
-      <c r="D20" s="14">
-        <v>7</v>
-      </c>
       <c r="E20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-7.5</v>
       </c>
       <c r="F20">
@@ -2088,37 +2032,42 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
+      <c r="I20" s="1">
+        <f t="shared" si="17"/>
+        <v>-3.5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>7</v>
+      </c>
       <c r="K20" s="11"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
-      <c r="P20" s="25"/>
+      <c r="P20" s="23"/>
       <c r="Q20" s="12"/>
       <c r="R20" s="13"/>
       <c r="S20" s="3"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-      <c r="X20" s="31" t="s">
+      <c r="X20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="31">
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29">
         <v>5</v>
       </c>
-      <c r="AE20" s="31" t="s">
+      <c r="AE20" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AF20" s="31"/>
-      <c r="AG20" s="33">
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="31">
         <f>AG21-AG22</f>
         <v>1.8301259941990371</v>
       </c>
-      <c r="AI20" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI20" s="18">
+        <f t="shared" si="18"/>
         <v>-1.8743915509016131</v>
       </c>
       <c r="AJ20">
@@ -2127,14 +2076,14 @@
       <c r="AK20">
         <v>1</v>
       </c>
-      <c r="AN20" s="35"/>
+      <c r="AN20" s="33"/>
       <c r="AQ20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="E21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-8.5</v>
       </c>
       <c r="F21">
@@ -2156,23 +2105,23 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-      <c r="X21" s="31" t="s">
+      <c r="X21" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Y21" s="31"/>
-      <c r="Z21" s="31">
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29">
         <v>0.20300000000000001</v>
       </c>
-      <c r="AE21" s="31" t="s">
+      <c r="AE21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="AF21" s="31"/>
-      <c r="AG21" s="33">
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="31">
         <f>MAX(AB11:AH16)</f>
         <v>-0.45096022208013986</v>
       </c>
-      <c r="AI21" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI21" s="18">
+        <f t="shared" si="18"/>
         <v>-1.6710442182128311</v>
       </c>
       <c r="AJ21">
@@ -2184,14 +2133,14 @@
       <c r="AM21">
         <v>2</v>
       </c>
-      <c r="AN21" s="35"/>
+      <c r="AN21" s="33"/>
       <c r="AP21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="E22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-9.5</v>
       </c>
       <c r="F22">
@@ -2219,24 +2168,24 @@
       <c r="Z22">
         <v>0</v>
       </c>
-      <c r="AA22" s="31" t="s">
+      <c r="AA22" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="AB22" s="31"/>
-      <c r="AC22" s="32">
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="30">
         <f>0-$Z$28+0.5</f>
         <v>-3.5</v>
       </c>
-      <c r="AE22" s="31" t="s">
+      <c r="AE22" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="33">
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="31">
         <f>MIN(AB12:AH17)</f>
         <v>-2.281086216279177</v>
       </c>
-      <c r="AI22" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI22" s="18">
+        <f t="shared" si="18"/>
         <v>-1.4676968855240493</v>
       </c>
       <c r="AJ22">
@@ -2251,7 +2200,7 @@
       <c r="AM22">
         <v>1</v>
       </c>
-      <c r="AN22" s="35"/>
+      <c r="AN22" s="33"/>
       <c r="AO22">
         <v>2</v>
       </c>
@@ -2264,7 +2213,7 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="E23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-10.5</v>
       </c>
       <c r="F23">
@@ -2292,53 +2241,53 @@
       <c r="Z23">
         <v>0</v>
       </c>
-      <c r="AA23" s="31" t="s">
+      <c r="AA23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="AB23" s="31"/>
-      <c r="AC23" s="32">
+      <c r="AB23" s="29"/>
+      <c r="AC23" s="30">
         <f>$Z$29-0-0.5</f>
         <v>3.5</v>
       </c>
-      <c r="AE23" s="31" t="s">
+      <c r="AE23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="AF23" s="31"/>
-      <c r="AG23" s="31">
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29">
         <v>10</v>
       </c>
-      <c r="AI23" s="34">
-        <f t="shared" si="23"/>
+      <c r="AI23" s="32">
+        <f t="shared" si="18"/>
         <v>-1.2643495528352675</v>
       </c>
-      <c r="AJ23" s="35">
+      <c r="AJ23" s="33">
         <v>5</v>
       </c>
-      <c r="AK23" s="35">
-        <v>1</v>
-      </c>
-      <c r="AL23" s="35">
-        <v>1</v>
-      </c>
-      <c r="AM23" s="35">
+      <c r="AK23" s="33">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="33">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="33">
         <v>2</v>
       </c>
-      <c r="AN23" s="35">
+      <c r="AN23" s="33">
         <v>6</v>
       </c>
-      <c r="AO23" s="35">
-        <v>1</v>
-      </c>
-      <c r="AP23" s="35">
-        <v>1</v>
-      </c>
-      <c r="AQ23" s="35">
+      <c r="AO23" s="33">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="33">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="E24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>-11.5</v>
       </c>
       <c r="F24">
@@ -2366,11 +2315,11 @@
       <c r="Z24">
         <v>7</v>
       </c>
-      <c r="AA24" s="31" t="s">
+      <c r="AA24" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="32">
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="30">
         <f>$Z$26-1-$Z$28+0.5</f>
         <v>3.5</v>
       </c>
@@ -2381,8 +2330,8 @@
         <f>Z19-Z18</f>
         <v>30</v>
       </c>
-      <c r="AI24" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI24" s="18">
+        <f t="shared" si="18"/>
         <v>-1.0610022201464855</v>
       </c>
       <c r="AJ24">
@@ -2408,24 +2357,24 @@
       <c r="Z25">
         <v>7</v>
       </c>
-      <c r="AA25" s="31" t="s">
+      <c r="AA25" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="32">
+      <c r="AB25" s="29"/>
+      <c r="AC25" s="30">
         <f>$Z$29-(Z27-1)-0.5</f>
         <v>-3.5</v>
       </c>
-      <c r="AE25" s="31" t="s">
+      <c r="AE25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="31">
+      <c r="AF25" s="29"/>
+      <c r="AG25" s="29">
         <f>AG24/Z20+1</f>
         <v>7</v>
       </c>
-      <c r="AI25" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI25" s="18">
+        <f t="shared" si="18"/>
         <v>-0.85765488745770369</v>
       </c>
       <c r="AJ25">
@@ -2462,8 +2411,8 @@
         <f>AG23*AG25</f>
         <v>70</v>
       </c>
-      <c r="AI26" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI26" s="18">
+        <f t="shared" si="18"/>
         <v>-0.65430755476892166</v>
       </c>
       <c r="AJ26">
@@ -2478,16 +2427,16 @@
         <f>Z25-Z23+1</f>
         <v>8</v>
       </c>
-      <c r="AE27" s="31" t="s">
+      <c r="AE27" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="AF27" s="31"/>
-      <c r="AG27" s="33">
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="31">
         <f>(AG21-AG22)/(AG23-1)</f>
         <v>0.20334733268878191</v>
       </c>
-      <c r="AI27" s="20">
-        <f t="shared" si="23"/>
+      <c r="AI27" s="18">
+        <f t="shared" si="18"/>
         <v>-0.45096022208013986</v>
       </c>
       <c r="AJ27">
@@ -2504,7 +2453,7 @@
       <c r="X28" t="s">
         <v>1</v>
       </c>
-      <c r="Z28" s="21">
+      <c r="Z28" s="19">
         <f>Z26/2</f>
         <v>4</v>
       </c>
@@ -2513,12 +2462,36 @@
       <c r="X29" t="s">
         <v>3</v>
       </c>
-      <c r="Z29" s="21">
+      <c r="Z29" s="19">
         <f>Z27/2</f>
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>3.5</v>
+      </c>
+      <c r="K30">
+        <v>2.5</v>
+      </c>
+      <c r="L30">
+        <v>1.5</v>
+      </c>
+      <c r="M30">
+        <v>0.5</v>
+      </c>
+      <c r="N30">
+        <v>-0.5</v>
+      </c>
+      <c r="O30">
+        <v>-1.5</v>
+      </c>
+      <c r="P30">
+        <v>-2.5</v>
+      </c>
+      <c r="Q30">
+        <v>-3.5</v>
+      </c>
       <c r="X30" t="s">
         <v>33</v>
       </c>
@@ -2526,33 +2499,68 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="H31">
-        <v>174</v>
-      </c>
-    </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="H32">
-        <f>H31*3.14159/180</f>
-        <v>3.0368703333333333</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33">
-        <f>COS(H32)</f>
-        <v>-0.99452162723519366</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34">
-        <f>SIN(H32)</f>
-        <v>0.10453101435202192</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35">
-        <f>57*H33+50*H34</f>
-        <v>-51.461182034804949</v>
+      <c r="J32">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="33" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>2.5</v>
+      </c>
+      <c r="L33">
+        <v>3.5</v>
+      </c>
+      <c r="M33">
+        <v>2.5</v>
+      </c>
+      <c r="N33">
+        <v>1.5</v>
+      </c>
+      <c r="O33">
+        <v>0.5</v>
+      </c>
+      <c r="P33">
+        <v>-0.5</v>
+      </c>
+      <c r="Q33">
+        <v>-1.5</v>
+      </c>
+      <c r="R33">
+        <v>-2.5</v>
+      </c>
+      <c r="S33">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="34" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>-3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>